<commit_message>
🚧: em progresso made by Caio Mizerkowski for college
</commit_message>
<xml_diff>
--- a/docs/plano_de_trabalho/Cronograma .xlsx
+++ b/docs/plano_de_trabalho/Cronograma .xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6DA9835-D28C-4670-8D42-C57C35E07B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ABA9CE0-5845-46A8-854B-F8C44CCAE5AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -277,12 +277,6 @@
     <t>Apresentação</t>
   </si>
   <si>
-    <t>TCC 1 - Problema inverso para a validação</t>
-  </si>
-  <si>
-    <t>TCC 2 - Analise de bijetividade do PA</t>
-  </si>
-  <si>
     <t>Desenvolvimento das rotinas</t>
   </si>
   <si>
@@ -316,6 +310,12 @@
   </si>
   <si>
     <t>Simulações e Análises</t>
+  </si>
+  <si>
+    <t>TCC 1 - Analise de bijetividade do PA</t>
+  </si>
+  <si>
+    <t>TCC 2 - Problema inverso para a validação</t>
   </si>
 </sst>
 </file>
@@ -1301,7 +1301,7 @@
     <xf numFmtId="1" fontId="11" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="11" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1374,44 +1374,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -2001,7 +2001,7 @@
   <dimension ref="A1:BM72"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="B4" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2055,77 +2055,77 @@
       <c r="B3" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="121" t="s">
+      <c r="C3" s="112" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="122"/>
-      <c r="E3" s="120">
+      <c r="D3" s="113"/>
+      <c r="E3" s="110">
         <f>BM4</f>
         <v>1</v>
       </c>
-      <c r="F3" s="120"/>
+      <c r="F3" s="110"/>
     </row>
     <row r="4" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="112" t="s">
-        <v>71</v>
-      </c>
-      <c r="I4" s="116" t="s">
+      <c r="B4" s="121" t="s">
+        <v>69</v>
+      </c>
+      <c r="I4" s="111" t="s">
         <v>43</v>
       </c>
-      <c r="J4" s="116"/>
-      <c r="K4" s="116"/>
-      <c r="L4" s="116"/>
-      <c r="M4" s="116" t="s">
+      <c r="J4" s="111"/>
+      <c r="K4" s="111"/>
+      <c r="L4" s="111"/>
+      <c r="M4" s="111" t="s">
         <v>44</v>
       </c>
-      <c r="N4" s="116"/>
-      <c r="O4" s="116"/>
-      <c r="P4" s="116"/>
-      <c r="Q4" s="116"/>
-      <c r="R4" s="116" t="s">
+      <c r="N4" s="111"/>
+      <c r="O4" s="111"/>
+      <c r="P4" s="111"/>
+      <c r="Q4" s="111"/>
+      <c r="R4" s="111" t="s">
         <v>45</v>
       </c>
-      <c r="S4" s="116"/>
-      <c r="T4" s="116"/>
-      <c r="U4" s="116"/>
-      <c r="V4" s="116" t="s">
+      <c r="S4" s="111"/>
+      <c r="T4" s="111"/>
+      <c r="U4" s="111"/>
+      <c r="V4" s="111" t="s">
         <v>46</v>
       </c>
-      <c r="W4" s="116"/>
-      <c r="X4" s="116"/>
-      <c r="Y4" s="116"/>
-      <c r="Z4" s="116" t="s">
+      <c r="W4" s="111"/>
+      <c r="X4" s="111"/>
+      <c r="Y4" s="111"/>
+      <c r="Z4" s="111" t="s">
         <v>47</v>
       </c>
-      <c r="AA4" s="116"/>
-      <c r="AB4" s="116"/>
-      <c r="AC4" s="116"/>
-      <c r="AD4" s="116"/>
-      <c r="AE4" s="116" t="s">
+      <c r="AA4" s="111"/>
+      <c r="AB4" s="111"/>
+      <c r="AC4" s="111"/>
+      <c r="AD4" s="111"/>
+      <c r="AE4" s="111" t="s">
         <v>48</v>
       </c>
-      <c r="AF4" s="116"/>
-      <c r="AG4" s="116"/>
-      <c r="AH4" s="116"/>
-      <c r="AI4" s="116" t="s">
+      <c r="AF4" s="111"/>
+      <c r="AG4" s="111"/>
+      <c r="AH4" s="111"/>
+      <c r="AI4" s="111" t="s">
         <v>49</v>
       </c>
-      <c r="AJ4" s="116"/>
-      <c r="AK4" s="116"/>
-      <c r="AL4" s="116"/>
-      <c r="AM4" s="117" t="s">
+      <c r="AJ4" s="111"/>
+      <c r="AK4" s="111"/>
+      <c r="AL4" s="111"/>
+      <c r="AM4" s="116" t="s">
         <v>62</v>
       </c>
-      <c r="AN4" s="118"/>
-      <c r="AO4" s="118"/>
-      <c r="AP4" s="118"/>
-      <c r="AQ4" s="119"/>
-      <c r="AR4" s="117" t="s">
+      <c r="AN4" s="117"/>
+      <c r="AO4" s="117"/>
+      <c r="AP4" s="117"/>
+      <c r="AQ4" s="118"/>
+      <c r="AR4" s="116" t="s">
         <v>50</v>
       </c>
-      <c r="AS4" s="118"/>
-      <c r="AT4" s="118"/>
-      <c r="AU4" s="119"/>
+      <c r="AS4" s="117"/>
+      <c r="AT4" s="117"/>
+      <c r="AU4" s="118"/>
       <c r="AV4" s="86"/>
       <c r="AW4" s="114"/>
       <c r="AX4" s="114"/>
@@ -2151,7 +2151,7 @@
       <c r="A5" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="113"/>
+      <c r="B5" s="122"/>
       <c r="C5" s="70"/>
       <c r="D5" s="70"/>
       <c r="E5" s="70"/>
@@ -2702,7 +2702,7 @@
         <v>37</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C8" s="56"/>
       <c r="D8" s="15"/>
@@ -2856,7 +2856,7 @@
         <v>38</v>
       </c>
       <c r="B10" s="65" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C10" s="57"/>
       <c r="D10" s="18">
@@ -3010,7 +3010,7 @@
     <row r="12" spans="1:65" s="3" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="48"/>
       <c r="B12" s="65" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C12" s="57"/>
       <c r="D12" s="18">
@@ -3232,13 +3232,13 @@
     </row>
     <row r="15" spans="1:65" s="3" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="48"/>
-      <c r="B15" s="110" t="s">
+      <c r="B15" s="119" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="110"/>
-      <c r="D15" s="110"/>
-      <c r="E15" s="110"/>
-      <c r="F15" s="110"/>
+      <c r="C15" s="119"/>
+      <c r="D15" s="119"/>
+      <c r="E15" s="119"/>
+      <c r="F15" s="119"/>
       <c r="G15" s="13"/>
       <c r="H15" s="13" t="str">
         <f t="shared" si="6"/>
@@ -3306,7 +3306,7 @@
         <v>39</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C16" s="58"/>
       <c r="D16" s="20"/>
@@ -3454,7 +3454,7 @@
     <row r="18" spans="1:64" s="3" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="48"/>
       <c r="B18" s="66" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C18" s="59"/>
       <c r="D18" s="21">
@@ -3608,7 +3608,7 @@
     <row r="20" spans="1:64" s="3" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="48"/>
       <c r="B20" s="66" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C20" s="59"/>
       <c r="D20" s="21">
@@ -3685,7 +3685,7 @@
     <row r="21" spans="1:64" s="3" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="48"/>
       <c r="B21" s="66" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C21" s="59"/>
       <c r="D21" s="21"/>
@@ -3828,13 +3828,13 @@
     </row>
     <row r="23" spans="1:64" s="3" customFormat="1" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="48"/>
-      <c r="B23" s="111" t="s">
+      <c r="B23" s="120" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="111"/>
-      <c r="D23" s="111"/>
-      <c r="E23" s="111"/>
-      <c r="F23" s="111"/>
+      <c r="C23" s="120"/>
+      <c r="D23" s="120"/>
+      <c r="E23" s="120"/>
+      <c r="F23" s="120"/>
       <c r="G23" s="13"/>
       <c r="H23" s="13" t="str">
         <f t="shared" si="6"/>
@@ -4917,16 +4917,16 @@
       <c r="V37" s="36"/>
       <c r="W37" s="36"/>
       <c r="X37" s="93" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="Y37" s="93" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="Z37" s="93" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AA37" s="93" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AB37" s="36"/>
       <c r="AC37" s="36"/>
@@ -4939,13 +4939,13 @@
       <c r="AJ37" s="36"/>
       <c r="AK37" s="36"/>
       <c r="AL37" s="93" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AM37" s="93" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AN37" s="93" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AO37" s="36"/>
       <c r="AP37" s="36"/>
@@ -5016,6 +5016,11 @@
     <row r="72" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="BA4:BD4"/>
+    <mergeCell ref="BE4:BH4"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="I4:L4"/>
     <mergeCell ref="C3:D3"/>
@@ -5029,11 +5034,6 @@
     <mergeCell ref="AI4:AL4"/>
     <mergeCell ref="AM4:AQ4"/>
     <mergeCell ref="AR4:AU4"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="BA4:BD4"/>
-    <mergeCell ref="BE4:BH4"/>
   </mergeCells>
   <phoneticPr fontId="25" type="noConversion"/>
   <conditionalFormatting sqref="D7:D13 D16:D22 D24:D37">

</xml_diff>